<commit_message>
Update sample data with tech-themed punny names
Replace generic employee names with tech/engineering themed pun names:
- Paige Duty (on-call duty)
- Lee Latency (performance obsessed)
- Mona Torr (monitoring dashboards)
- Robin Rollback (deployment rescue)
- Kenny Canary (canary deployments)
- And 45 more creative tech puns!

These names make the demo data more fun and memorable while
maintaining the same realistic distribution of roles, departments,
and salary ranges.

Names created by: Gemini Pro 3

🤖 Generated with Claude Code (https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data.xlsx
+++ b/sample-data.xlsx
@@ -521,7 +521,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alice Anderson</t>
+          <t>Paige Duty</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>151000</v>
+        <v>146000</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -561,7 +561,7 @@
         <v>95</v>
       </c>
       <c r="M3" t="n">
-        <v>18120</v>
+        <v>17520</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
@@ -569,7 +569,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bob Brown</t>
+          <t>Lee Latency</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>100000</v>
+        <v>97000</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -606,10 +606,10 @@
         <v>10</v>
       </c>
       <c r="L4" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="M4" t="n">
-        <v>10000</v>
+        <v>9700</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
@@ -617,7 +617,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Carol Chen</t>
+          <t>Mona Torr</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>215000</v>
+        <v>205000</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -653,11 +653,8 @@
       <c r="K5" t="n">
         <v>15</v>
       </c>
-      <c r="L5" t="n">
-        <v>105</v>
-      </c>
       <c r="M5" t="n">
-        <v>32250</v>
+        <v>30750</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
@@ -665,7 +662,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>David Davis</t>
+          <t>Robin Rollback</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -686,7 +683,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>155000</v>
+        <v>152000</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -702,10 +699,10 @@
         <v>12</v>
       </c>
       <c r="L6" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="M6" t="n">
-        <v>18600</v>
+        <v>18240</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
@@ -713,7 +710,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Emma Evans</t>
+          <t>Kenny Canary</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -734,7 +731,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>266000</v>
+        <v>258000</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -750,7 +747,7 @@
         <v>20</v>
       </c>
       <c r="M7" t="n">
-        <v>53200</v>
+        <v>51600</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
@@ -758,7 +755,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Frank Foster</t>
+          <t>Tracey Loggins</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -779,7 +776,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>147000</v>
+        <v>142000</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -795,10 +792,10 @@
         <v>12</v>
       </c>
       <c r="L8" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="M8" t="n">
-        <v>17640</v>
+        <v>17040</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
@@ -806,7 +803,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Grace Garcia</t>
+          <t>Sue Q. Ell</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -827,7 +824,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>110000</v>
+        <v>117000</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -843,10 +840,10 @@
         <v>10</v>
       </c>
       <c r="L9" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M9" t="n">
-        <v>11000</v>
+        <v>11700</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
@@ -854,7 +851,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Henry Harris</t>
+          <t>Jason Blob</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -875,7 +872,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>137000</v>
+        <v>169000</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -890,8 +887,11 @@
       <c r="K10" t="n">
         <v>12</v>
       </c>
+      <c r="L10" t="n">
+        <v>105</v>
+      </c>
       <c r="M10" t="n">
-        <v>16440</v>
+        <v>20280</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
@@ -899,7 +899,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Iris Ibrahim</t>
+          <t>Al Ert</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>175000</v>
+        <v>190000</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -935,11 +935,8 @@
       <c r="K11" t="n">
         <v>15</v>
       </c>
-      <c r="L11" t="n">
-        <v>95</v>
-      </c>
       <c r="M11" t="n">
-        <v>26250</v>
+        <v>28500</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
@@ -947,7 +944,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jack Johnson</t>
+          <t>Addie Min</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -968,7 +965,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>151000</v>
+        <v>144000</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -984,10 +981,10 @@
         <v>12</v>
       </c>
       <c r="L12" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="M12" t="n">
-        <v>18120</v>
+        <v>17280</v>
       </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
@@ -995,7 +992,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kelly Kim</t>
+          <t>Tim Out</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1016,7 +1013,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>160000</v>
+        <v>162000</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1032,10 +1029,10 @@
         <v>12</v>
       </c>
       <c r="L13" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M13" t="n">
-        <v>19200</v>
+        <v>19440</v>
       </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
@@ -1043,7 +1040,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Liam Lee</t>
+          <t>Barbie Que</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1064,7 +1061,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>92000</v>
+        <v>98000</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1080,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="M14" t="n">
-        <v>9200</v>
+        <v>9800</v>
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
@@ -1088,7 +1085,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Maya Martinez</t>
+          <t>Terry Byte</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1109,7 +1106,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>163000</v>
+        <v>152000</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1125,10 +1122,10 @@
         <v>12</v>
       </c>
       <c r="L15" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M15" t="n">
-        <v>19560</v>
+        <v>18240</v>
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
@@ -1136,7 +1133,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Noah Nguyen</t>
+          <t>Nole Pointer</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1157,7 +1154,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>196000</v>
+        <v>219000</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1172,8 +1169,11 @@
       <c r="K16" t="n">
         <v>15</v>
       </c>
+      <c r="L16" t="n">
+        <v>100</v>
+      </c>
       <c r="M16" t="n">
-        <v>29400</v>
+        <v>32850</v>
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
@@ -1181,7 +1181,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Olivia O'Brien</t>
+          <t>Marge Conflict</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>170000</v>
+        <v>138000</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         <v>12</v>
       </c>
       <c r="L17" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="M17" t="n">
-        <v>20400</v>
+        <v>16560</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
@@ -1229,7 +1229,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Peter Patel</t>
+          <t>Bridget Branch</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>115000</v>
+        <v>97000</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1265,11 +1265,8 @@
       <c r="K18" t="n">
         <v>10</v>
       </c>
-      <c r="L18" t="n">
-        <v>110</v>
-      </c>
       <c r="M18" t="n">
-        <v>11500</v>
+        <v>9700</v>
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
@@ -1277,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Quinn Quinn</t>
+          <t>Cody Ryder</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1298,7 +1295,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>188000</v>
+        <v>187000</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1313,8 +1310,11 @@
       <c r="K19" t="n">
         <v>15</v>
       </c>
+      <c r="L19" t="n">
+        <v>105</v>
+      </c>
       <c r="M19" t="n">
-        <v>28200</v>
+        <v>28050</v>
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
@@ -1322,7 +1322,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Rachel Rodriguez</t>
+          <t>Cy Ferr</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>116000</v>
+        <v>119000</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1359,10 +1359,10 @@
         <v>12</v>
       </c>
       <c r="L20" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="M20" t="n">
-        <v>13920</v>
+        <v>14280</v>
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
@@ -1370,7 +1370,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sam Smith</t>
+          <t>Phil Wall</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>182000</v>
+        <v>166000</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         <v>15</v>
       </c>
       <c r="M21" t="n">
-        <v>27300</v>
+        <v>24900</v>
       </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
@@ -1415,7 +1415,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Taylor Taylor</t>
+          <t>Lana Wan</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1436,7 +1436,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>138000</v>
+        <v>169000</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1452,10 +1452,10 @@
         <v>12</v>
       </c>
       <c r="L22" t="n">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="M22" t="n">
-        <v>16560</v>
+        <v>20280</v>
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
@@ -1463,7 +1463,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Uma Usman</t>
+          <t>Artie Ficial</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1484,7 +1484,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>103000</v>
+        <v>121000</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1499,11 +1499,8 @@
       <c r="K23" t="n">
         <v>10</v>
       </c>
-      <c r="L23" t="n">
-        <v>110</v>
-      </c>
       <c r="M23" t="n">
-        <v>10300</v>
+        <v>12100</v>
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
@@ -1511,7 +1508,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Victor Vargas</t>
+          <t>Ruth Cause</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1532,7 +1529,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>140000</v>
+        <v>170000</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1547,8 +1544,11 @@
       <c r="K24" t="n">
         <v>12</v>
       </c>
+      <c r="L24" t="n">
+        <v>95</v>
+      </c>
       <c r="M24" t="n">
-        <v>16800</v>
+        <v>20400</v>
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
@@ -1556,7 +1556,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Wendy Williams</t>
+          <t>Matt Rick</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>100000</v>
+        <v>96000</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1593,10 +1593,10 @@
         <v>10</v>
       </c>
       <c r="L25" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M25" t="n">
-        <v>10000</v>
+        <v>9600</v>
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
@@ -1604,7 +1604,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Xavier Xavier</t>
+          <t>Cassie Cache</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>177000</v>
+        <v>143000</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1640,11 +1640,8 @@
       <c r="K26" t="n">
         <v>12</v>
       </c>
-      <c r="L26" t="n">
-        <v>100</v>
-      </c>
       <c r="M26" t="n">
-        <v>21240</v>
+        <v>17160</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
@@ -1652,7 +1649,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Yara Yang</t>
+          <t>Sue Do</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1673,7 +1670,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>100000</v>
+        <v>126000</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1688,11 +1685,8 @@
       <c r="K27" t="n">
         <v>10</v>
       </c>
-      <c r="L27" t="n">
-        <v>90</v>
-      </c>
       <c r="M27" t="n">
-        <v>10000</v>
+        <v>12600</v>
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
@@ -1700,7 +1694,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Zoe Zhang</t>
+          <t>Pat Ch</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1721,7 +1715,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>123000</v>
+        <v>142000</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1737,10 +1731,10 @@
         <v>10</v>
       </c>
       <c r="L28" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="M28" t="n">
-        <v>12300</v>
+        <v>14200</v>
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
@@ -1748,7 +1742,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alex Ahmed</t>
+          <t>Devin Null</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1769,7 +1763,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>99000</v>
+        <v>98000</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1784,11 +1778,8 @@
       <c r="K29" t="n">
         <v>8</v>
       </c>
-      <c r="L29" t="n">
-        <v>95</v>
-      </c>
       <c r="M29" t="n">
-        <v>7920</v>
+        <v>7840</v>
       </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
@@ -1796,7 +1787,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Blake Baker</t>
+          <t>Justin Time</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1817,7 +1808,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>96000</v>
+        <v>91000</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1836,7 +1827,7 @@
         <v>110</v>
       </c>
       <c r="M30" t="n">
-        <v>7680</v>
+        <v>7280</v>
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
@@ -1844,7 +1835,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Casey Cohen</t>
+          <t>Annie O'Maly</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1865,7 +1856,7 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>130000</v>
+        <v>154000</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1880,11 +1871,8 @@
       <c r="K31" t="n">
         <v>12</v>
       </c>
-      <c r="L31" t="n">
-        <v>100</v>
-      </c>
       <c r="M31" t="n">
-        <v>15600</v>
+        <v>18480</v>
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
@@ -1892,7 +1880,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Drew Diaz</t>
+          <t>Sam Box</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1940,7 +1928,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ella Ellis</t>
+          <t>Val Idation</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1961,7 +1949,7 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>99000</v>
+        <v>102000</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1976,8 +1964,11 @@
       <c r="K33" t="n">
         <v>10</v>
       </c>
+      <c r="L33" t="n">
+        <v>115</v>
+      </c>
       <c r="M33" t="n">
-        <v>9900</v>
+        <v>10200</v>
       </c>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
@@ -1985,7 +1976,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Finn Fischer</t>
+          <t>Bill Ding</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2006,7 +1997,7 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>91000</v>
+        <v>104000</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2021,8 +2012,11 @@
       <c r="K34" t="n">
         <v>10</v>
       </c>
+      <c r="L34" t="n">
+        <v>90</v>
+      </c>
       <c r="M34" t="n">
-        <v>9100</v>
+        <v>10400</v>
       </c>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
@@ -2030,7 +2024,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Gia Green</t>
+          <t>Ty Po</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2051,7 +2045,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>169000</v>
+        <v>152000</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2070,7 +2064,7 @@
         <v>115</v>
       </c>
       <c r="M35" t="n">
-        <v>20280</v>
+        <v>18240</v>
       </c>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
@@ -2078,7 +2072,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Harper Hill</t>
+          <t>Mike Roservices</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2099,7 +2093,7 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>149000</v>
+        <v>150000</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2118,7 +2112,7 @@
         <v>100</v>
       </c>
       <c r="M36" t="n">
-        <v>17880</v>
+        <v>18000</v>
       </c>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
@@ -2126,7 +2120,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ivan Islam</t>
+          <t>Lou Pe</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2147,7 +2141,7 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>135000</v>
+        <v>147000</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2163,7 +2157,7 @@
         <v>12</v>
       </c>
       <c r="M37" t="n">
-        <v>16200</v>
+        <v>17640</v>
       </c>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
@@ -2171,7 +2165,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jules Jones</t>
+          <t>Connie Tainer</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2192,7 +2186,7 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>120000</v>
+        <v>138000</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2207,8 +2201,11 @@
       <c r="K38" t="n">
         <v>12</v>
       </c>
+      <c r="L38" t="n">
+        <v>100</v>
+      </c>
       <c r="M38" t="n">
-        <v>14400</v>
+        <v>16560</v>
       </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
@@ -2216,7 +2213,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Kai Khan</t>
+          <t>Noah Node</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2237,7 +2234,7 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>95000</v>
+        <v>93000</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2253,10 +2250,10 @@
         <v>8</v>
       </c>
       <c r="L39" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="M39" t="n">
-        <v>7600</v>
+        <v>7440</v>
       </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
@@ -2264,7 +2261,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Luna Lopez</t>
+          <t>Sara Ver</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2312,7 +2309,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Max Miller</t>
+          <t>Exa M. Elle</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2333,10 +2330,10 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>100330</v>
+        <v>99540</v>
       </c>
       <c r="H41" t="n">
-        <v>127000</v>
+        <v>126000</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2351,14 +2348,11 @@
       <c r="K41" t="n">
         <v>10</v>
       </c>
-      <c r="L41" t="n">
-        <v>100</v>
-      </c>
       <c r="M41" t="n">
-        <v>10033</v>
+        <v>9954</v>
       </c>
       <c r="N41" t="n">
-        <v>12700</v>
+        <v>12600</v>
       </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
@@ -2366,7 +2360,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Nora Nelson</t>
+          <t>Dee Ploi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2387,14 +2381,14 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>118800</v>
+        <v>83740</v>
       </c>
       <c r="H42" t="n">
-        <v>88000</v>
+        <v>106000</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -2406,13 +2400,13 @@
         <v>8</v>
       </c>
       <c r="L42" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="M42" t="n">
-        <v>9504</v>
+        <v>6699.200000000001</v>
       </c>
       <c r="N42" t="n">
-        <v>7040</v>
+        <v>8480</v>
       </c>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr"/>
@@ -2420,7 +2414,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Owen Okafor</t>
+          <t>Ray D. O'Button</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2441,14 +2435,14 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>9075000</v>
+        <v>98440</v>
       </c>
       <c r="H43" t="n">
-        <v>110000</v>
+        <v>107000</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2459,14 +2453,11 @@
       <c r="K43" t="n">
         <v>10</v>
       </c>
-      <c r="L43" t="n">
-        <v>85</v>
-      </c>
       <c r="M43" t="n">
-        <v>907500</v>
+        <v>9844</v>
       </c>
       <c r="N43" t="n">
-        <v>11000</v>
+        <v>10700</v>
       </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
@@ -2474,7 +2465,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Piper Park</t>
+          <t>Cam Elcase</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2495,14 +2486,14 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>153640</v>
+        <v>107440</v>
       </c>
       <c r="H44" t="n">
-        <v>167000</v>
+        <v>136000</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -2513,14 +2504,11 @@
       <c r="K44" t="n">
         <v>12</v>
       </c>
-      <c r="L44" t="n">
-        <v>100</v>
-      </c>
       <c r="M44" t="n">
-        <v>18436.8</v>
+        <v>12892.8</v>
       </c>
       <c r="N44" t="n">
-        <v>20040</v>
+        <v>16320</v>
       </c>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr"/>
@@ -2528,7 +2516,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Rowan Rossi</t>
+          <t>Hashim Map</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2549,14 +2537,14 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>205200</v>
+        <v>13530000</v>
       </c>
       <c r="H45" t="n">
-        <v>152000</v>
+        <v>164000</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>INR</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2567,14 +2555,11 @@
       <c r="K45" t="n">
         <v>12</v>
       </c>
-      <c r="L45" t="n">
-        <v>85</v>
-      </c>
       <c r="M45" t="n">
-        <v>24624</v>
+        <v>1623600</v>
       </c>
       <c r="N45" t="n">
-        <v>18240</v>
+        <v>19680</v>
       </c>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr"/>
@@ -2582,7 +2567,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sage Santos</t>
+          <t>Ben Chmark</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2603,14 +2588,14 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>157950</v>
+        <v>8002500</v>
       </c>
       <c r="H46" t="n">
-        <v>117000</v>
+        <v>97000</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>INR</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2621,11 +2606,14 @@
       <c r="K46" t="n">
         <v>10</v>
       </c>
+      <c r="L46" t="n">
+        <v>85</v>
+      </c>
       <c r="M46" t="n">
-        <v>15795</v>
+        <v>800250</v>
       </c>
       <c r="N46" t="n">
-        <v>11700</v>
+        <v>9700</v>
       </c>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr"/>
@@ -2633,7 +2621,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Tess Thomas</t>
+          <t>Grace Full</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2654,10 +2642,10 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>106650</v>
+        <v>105070</v>
       </c>
       <c r="H47" t="n">
-        <v>135000</v>
+        <v>133000</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2673,13 +2661,13 @@
         <v>12</v>
       </c>
       <c r="L47" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="M47" t="n">
-        <v>12798</v>
+        <v>12608.4</v>
       </c>
       <c r="N47" t="n">
-        <v>16200</v>
+        <v>15960</v>
       </c>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr"/>
@@ -2687,7 +2675,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Uri Underwood</t>
+          <t>Shel Script</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2708,14 +2696,14 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>142600</v>
+        <v>12705000</v>
       </c>
       <c r="H48" t="n">
-        <v>155000</v>
+        <v>154000</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>INR</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2726,11 +2714,14 @@
       <c r="K48" t="n">
         <v>15</v>
       </c>
+      <c r="L48" t="n">
+        <v>100</v>
+      </c>
       <c r="M48" t="n">
-        <v>21390</v>
+        <v>1905750</v>
       </c>
       <c r="N48" t="n">
-        <v>23250</v>
+        <v>23100</v>
       </c>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr"/>
@@ -2738,7 +2729,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Vale Vasquez</t>
+          <t>Sal T. Hash</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2759,10 +2750,10 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>217350</v>
+        <v>226800</v>
       </c>
       <c r="H49" t="n">
-        <v>161000</v>
+        <v>168000</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -2777,14 +2768,11 @@
       <c r="K49" t="n">
         <v>12</v>
       </c>
-      <c r="L49" t="n">
-        <v>115</v>
-      </c>
       <c r="M49" t="n">
-        <v>26082</v>
+        <v>27216</v>
       </c>
       <c r="N49" t="n">
-        <v>19320</v>
+        <v>20160</v>
       </c>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr"/>
@@ -2792,7 +2780,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Wade Wilson</t>
+          <t>Reba Boot</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2813,10 +2801,10 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>12127500</v>
+        <v>12622500</v>
       </c>
       <c r="H50" t="n">
-        <v>147000</v>
+        <v>153000</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2831,14 +2819,11 @@
       <c r="K50" t="n">
         <v>12</v>
       </c>
-      <c r="L50" t="n">
-        <v>100</v>
-      </c>
       <c r="M50" t="n">
-        <v>1455300</v>
+        <v>1514700</v>
       </c>
       <c r="N50" t="n">
-        <v>17640</v>
+        <v>18360</v>
       </c>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr"/>
@@ -2846,7 +2831,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Xena Xu</t>
+          <t>Stan Dup</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2867,14 +2852,14 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>13035000</v>
+        <v>135880</v>
       </c>
       <c r="H51" t="n">
-        <v>158000</v>
+        <v>172000</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -2886,13 +2871,13 @@
         <v>12</v>
       </c>
       <c r="L51" t="n">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="M51" t="n">
-        <v>1564200</v>
+        <v>16305.6</v>
       </c>
       <c r="N51" t="n">
-        <v>18960</v>
+        <v>20640</v>
       </c>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr"/>
@@ -2900,7 +2885,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Yale Yilmaz</t>
+          <t>Kay Eight</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2921,14 +2906,14 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>126960</v>
+        <v>10807500</v>
       </c>
       <c r="H52" t="n">
-        <v>138000</v>
+        <v>131000</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>INR</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -2940,13 +2925,13 @@
         <v>10</v>
       </c>
       <c r="L52" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M52" t="n">
-        <v>12696</v>
+        <v>1080750</v>
       </c>
       <c r="N52" t="n">
-        <v>13800</v>
+        <v>13100</v>
       </c>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr"/>

</xml_diff>